<commit_message>
added excel import feature.
</commit_message>
<xml_diff>
--- a/persistence/src/test/resources/file-import.xlsx
+++ b/persistence/src/test/resources/file-import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ionut/work/yali-mis/persistence/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ionut/work/dg-toolkit/persistence/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{6BC9B3DB-877C-4043-95A0-B6C42078F822}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8480CB0A-9367-764D-B839-B1DEAC62298E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>